<commit_message>
adding some change in checkbox and excel epmplyee
</commit_message>
<xml_diff>
--- a/src/assets/sample/employee.xlsx
+++ b/src/assets/sample/employee.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yas\Desktop\Doc\one\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>وضعیت</t>
   </si>
@@ -212,13 +212,22 @@
   </si>
   <si>
     <t>barati@yahoos.com</t>
+  </si>
+  <si>
+    <t>0020123448</t>
+  </si>
+  <si>
+    <t>0020123447</t>
+  </si>
+  <si>
+    <t>09123456789</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,6 +355,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,31 +669,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="4" width="45.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="9" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" style="2" customWidth="1"/>
     <col min="6" max="7" width="46.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="35.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -696,18 +714,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
-      <c r="B2" s="1">
-        <v>15527422962</v>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
-        <v>93580505122</v>
+      <c r="D2" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>16</v>
@@ -728,18 +746,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
-      <c r="B3" s="1">
-        <v>1252845262</v>
+      <c r="B3" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
-        <v>912555266</v>
+      <c r="D3" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>17</v>
@@ -760,187 +778,187 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="18">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="18">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="18">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="18">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="18">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="18">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="18">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="18">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="18">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="18">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="18">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="18">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="18">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="18">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="18">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="18">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="18">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>

</xml_diff>